<commit_message>
6.1, tang ca 12
</commit_message>
<xml_diff>
--- a/static/uploads/mau/dieuchuyen/dieuchuyen.xlsx
+++ b/static/uploads/mau/dieuchuyen/dieuchuyen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khanh\Desktop\Phần mềm Nam Thuận\HRM\static\uploads\mau\dieuchuyen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{365A2EE6-B383-4991-B3C3-C8249591CAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17D4B09-1BF9-44B3-B549-48101BD152E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9B5930FA-5E56-4E11-B87B-5466E15E00BC}"/>
   </bookViews>
@@ -34,83 +34,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
-  <si>
-    <t>Nhà máy</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Mã số thẻ</t>
   </si>
   <si>
-    <t>Họ tên</t>
-  </si>
-  <si>
-    <t>Chức danh cũ</t>
-  </si>
-  <si>
     <t>Chức danh mới</t>
   </si>
   <si>
-    <t>Chuyền cũ</t>
-  </si>
-  <si>
     <t>Chuyền mới</t>
   </si>
   <si>
-    <t>Chức danh TA cũ</t>
-  </si>
-  <si>
-    <t>Chức danh TA mới</t>
-  </si>
-  <si>
-    <t>Cấp bậc cũ</t>
-  </si>
-  <si>
-    <t>Cấp bậc mới</t>
-  </si>
-  <si>
-    <t>Section code cũ</t>
-  </si>
-  <si>
-    <t>Section code mới</t>
-  </si>
-  <si>
-    <t>Section description cũ</t>
-  </si>
-  <si>
-    <t>Section description mới</t>
-  </si>
-  <si>
-    <t>HC category cũ</t>
-  </si>
-  <si>
-    <t>HC category mới</t>
-  </si>
-  <si>
-    <t>Phòng ban cũ</t>
-  </si>
-  <si>
-    <t>Phòng ban mới</t>
-  </si>
-  <si>
-    <t>Employee type cũ</t>
-  </si>
-  <si>
-    <t>Employee type mới</t>
-  </si>
-  <si>
-    <t>Position code cũ</t>
-  </si>
-  <si>
-    <t>Position code mới</t>
-  </si>
-  <si>
-    <t>Position code description cũ</t>
-  </si>
-  <si>
-    <t>Position code description mới</t>
-  </si>
-  <si>
     <t>Loại điều chuyển</t>
   </si>
   <si>
@@ -120,55 +54,13 @@
     <t>Ghi chú</t>
   </si>
   <si>
-    <t>NT1</t>
-  </si>
-  <si>
     <t>Công nhân may công nghiệp</t>
   </si>
   <si>
-    <t>11S13</t>
-  </si>
-  <si>
     <t>12S01</t>
   </si>
   <si>
-    <t>Sùng Thị Giàng</t>
-  </si>
-  <si>
     <t>Chuyển vị trí</t>
-  </si>
-  <si>
-    <t>Sewer</t>
-  </si>
-  <si>
-    <t>W1</t>
-  </si>
-  <si>
-    <t>1P01</t>
-  </si>
-  <si>
-    <t>1SEW1</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>1PDN</t>
-  </si>
-  <si>
-    <t>Incentive Worker</t>
-  </si>
-  <si>
-    <t>SWR</t>
-  </si>
-  <si>
-    <t>Skilled worker</t>
-  </si>
-  <si>
-    <t>1P02</t>
-  </si>
-  <si>
-    <t>1SEW2</t>
   </si>
 </sst>
 </file>
@@ -193,15 +85,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -209,17 +107,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -536,208 +452,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20ECFE8D-7C58-4856-942F-B682F50F7DE1}">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="R3" sqref="A3:XFD42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="28" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>13295</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2">
-        <v>13295</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R2" t="s">
-        <v>39</v>
-      </c>
-      <c r="S2" t="s">
-        <v>39</v>
-      </c>
-      <c r="T2" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" t="s">
-        <v>40</v>
-      </c>
-      <c r="V2" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" t="s">
-        <v>41</v>
-      </c>
-      <c r="X2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA2" s="2">
+      <c r="E2" s="2">
         <v>45516</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sửa file điều chuyển: chọn loại điều chọn chứ không nhập tay
</commit_message>
<xml_diff>
--- a/static/uploads/mau/dieuchuyen/dieuchuyen.xlsx
+++ b/static/uploads/mau/dieuchuyen/dieuchuyen.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khanh\Desktop\Phần mềm Nam Thuận\HRM\static\uploads\mau\dieuchuyen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Phanmem\HRM\static\uploads\mau\dieuchuyen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17D4B09-1BF9-44B3-B549-48101BD152E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9B5930FA-5E56-4E11-B87B-5466E15E00BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Mã số thẻ</t>
   </si>
@@ -61,12 +61,24 @@
   </si>
   <si>
     <t>Chuyển vị trí</t>
+  </si>
+  <si>
+    <t>Nghỉ việc</t>
+  </si>
+  <si>
+    <t>Nghỉ thai sản</t>
+  </si>
+  <si>
+    <t>Thai sản đi làm lại</t>
+  </si>
+  <si>
+    <t>Rút hồ sơ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -451,11 +463,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20ECFE8D-7C58-4856-942F-B682F50F7DE1}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,6 +517,70 @@
         <v>45516</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>12543</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2">
+        <v>45519</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$1:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D70</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>